<commit_message>
added (created at) time for the targets
</commit_message>
<xml_diff>
--- a/Features backlog.xlsx
+++ b/Features backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SalehRam\Desktop\Projects\Python\astroplanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D83E92-5BD8-4FE3-BED7-F45E67395DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F29F27-7F22-4932-AD4F-B9CFFC7136F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,12 +78,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,9 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +405,7 @@
   <dimension ref="B2:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,7 +434,7 @@
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -423,12 +444,12 @@
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -438,7 +459,7 @@
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>